<commit_message>
Adding examples/QA fixes/DT01 test cases and updated bundle
</commit_message>
<xml_diff>
--- a/input/l2/ANC Test Cases.xlsx
+++ b/input/l2/ANC Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryn\Documents\Src\WHO\anc-cds\input\l2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8290E5B1-A8A9-4E03-8716-42FFFDB61F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DF7550-4E20-4D4C-8316-B10A17F6D2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2595" yWindow="3195" windowWidth="18900" windowHeight="12015" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -2295,11 +2295,11 @@
   </sheetPr>
   <dimension ref="A1:ED1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="CM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomRight" activeCell="AQ2" sqref="AQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30075,7 +30075,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD945E7-B5AB-41D2-B981-9EA04595E329}">
   <dimension ref="A1:C128"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -30471,7 +30473,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>